<commit_message>
modified:   event_calendar.py 	modified:   event_items.py 	modified:   main.py 	modified:   "\345\256\266\346\227\217\346\210\220\345\221\230\346\230\257\345\220\246\345\234\250\347\276\244.xlsx"
</commit_message>
<xml_diff>
--- a/家族成员是否在群.xlsx
+++ b/家族成员是否在群.xlsx
@@ -5,18 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyf13\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zyf13\Desktop\科学修仙\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8B3314E-6213-46CB-BDD9-E01080CADAB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0C9DF28-6F32-462D-A78B-7A80D072F7A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="16491" yWindow="4414" windowWidth="15258" windowHeight="13055" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14691" yWindow="1269" windowWidth="15258" windowHeight="13054" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$C$1:$C$45</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="48">
   <si>
     <t xml:space="preserve"> 仙`从容</t>
   </si>
@@ -99,12 +99,6 @@
     <t xml:space="preserve"> 黄河`叮咚猫</t>
   </si>
   <si>
-    <t xml:space="preserve"> Fine (不知道是谁)</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 黄河`笑语</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 仙`二拐</t>
   </si>
   <si>
@@ -153,12 +147,6 @@
     <t xml:space="preserve"> 仙`荒天帝</t>
   </si>
   <si>
-    <t xml:space="preserve"> 黄河`星海</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 仙`悟空</t>
-  </si>
-  <si>
     <t>玩家</t>
   </si>
   <si>
@@ -172,6 +160,18 @@
   </si>
   <si>
     <t>是否在群里</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 仙`凌寒</t>
+  </si>
+  <si>
+    <t>仙`清酒</t>
+  </si>
+  <si>
+    <t>仙`烟熏柿子</t>
+  </si>
+  <si>
+    <t>仙`龙竹</t>
   </si>
 </sst>
 </file>
@@ -495,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C44"/>
+  <dimension ref="A1:C46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -509,13 +509,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.4">
@@ -526,7 +526,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.4">
@@ -537,7 +537,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.4">
@@ -548,7 +548,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.4">
@@ -559,7 +559,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.4">
@@ -567,9 +567,6 @@
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
         <v>45</v>
       </c>
     </row>
@@ -578,10 +575,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.4">
@@ -589,10 +586,10 @@
         <v>7</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.4">
@@ -600,10 +597,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.4">
@@ -611,10 +608,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.4">
@@ -622,10 +619,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.4">
@@ -633,366 +630,366 @@
         <v>11</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A16" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A18" s="2">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A19" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A20" s="2">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A21" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A22" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>20</v>
+        <v>44</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A23" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A24" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A25" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A26" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A27" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>25</v>
+        <v>37</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A28" s="2">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>26</v>
+        <v>46</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A29" s="2">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>27</v>
+        <v>35</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A30" s="2">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A31" s="2">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A32" s="2">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A33" s="2">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A34" s="2">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>32</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A35" s="2">
-        <v>35</v>
-      </c>
-      <c r="B35" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.4">
-      <c r="A36" s="2">
-        <v>36</v>
-      </c>
-      <c r="B36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A37" s="2">
-        <v>37</v>
+        <v>1</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A38" s="2">
-        <v>38</v>
+        <v>2</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A39" s="2">
-        <v>39</v>
+        <v>3</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A40" s="2">
-        <v>40</v>
+        <v>4</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A41" s="2">
-        <v>41</v>
+        <v>5</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>39</v>
+        <v>28</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A42" s="2">
+        <v>6</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B42" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A43" s="2">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.4">
       <c r="A44" s="2">
-        <v>44</v>
+        <v>9</v>
       </c>
       <c r="B44" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C44" s="1" t="s">
-        <v>46</v>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A45" s="2">
+        <v>10</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.4">
+      <c r="A46" s="2">
+        <v>11</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C44" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="C1:C42" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>